<commit_message>
deleted some extra files
</commit_message>
<xml_diff>
--- a/ConsoleApp1/bin/Debug/net8.0/123.xlsx
+++ b/ConsoleApp1/bin/Debug/net8.0/123.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notso\OneDrive\Desktop\GitHub\APRIORI\ConsoleApp1\bin\Debug\net8.0\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44530E6A-C412-4E6A-B659-7C1A095C95B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="10">
+  <si>
+    <t>ID_клиента</t>
+  </si>
+  <si>
+    <t>Кредитная_история</t>
+  </si>
+  <si>
+    <t>Возраст</t>
+  </si>
+  <si>
+    <t>Доход</t>
+  </si>
+  <si>
+    <t>Статус_занятости</t>
+  </si>
+  <si>
+    <t>Тип_продукта</t>
+  </si>
+  <si>
+    <t>Отличная</t>
+  </si>
+  <si>
+    <t>Полная</t>
+  </si>
+  <si>
+    <t>Ипотека</t>
+  </si>
+  <si>
+    <t>Плохая</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +69,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,11 +121,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +414,519 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:F25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
+        <v>70</v>
+      </c>
+      <c r="D2" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>70</v>
+      </c>
+      <c r="D3" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>70</v>
+      </c>
+      <c r="D4" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>70</v>
+      </c>
+      <c r="D5" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>70</v>
+      </c>
+      <c r="D6" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>70</v>
+      </c>
+      <c r="D7" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2">
+        <v>70</v>
+      </c>
+      <c r="D8" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>70</v>
+      </c>
+      <c r="D9" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2">
+        <v>70</v>
+      </c>
+      <c r="D10" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2">
+        <v>70</v>
+      </c>
+      <c r="D11" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2">
+        <v>70</v>
+      </c>
+      <c r="D12" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2">
+        <v>70</v>
+      </c>
+      <c r="D13" s="2">
+        <v>60000</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2">
+        <v>69</v>
+      </c>
+      <c r="D14" s="2">
+        <v>60001</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>69</v>
+      </c>
+      <c r="D15" s="2">
+        <v>60002</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2">
+        <v>69</v>
+      </c>
+      <c r="D16" s="2">
+        <v>60003</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2">
+        <v>69</v>
+      </c>
+      <c r="D17" s="2">
+        <v>60004</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2">
+        <v>60005</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2">
+        <v>69</v>
+      </c>
+      <c r="D19" s="2">
+        <v>60006</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2">
+        <v>69</v>
+      </c>
+      <c r="D20" s="2">
+        <v>60007</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2">
+        <v>69</v>
+      </c>
+      <c r="D21" s="2">
+        <v>60008</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2">
+        <v>69</v>
+      </c>
+      <c r="D22" s="2">
+        <v>60009</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2">
+        <v>69</v>
+      </c>
+      <c r="D23" s="2">
+        <v>60010</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2">
+        <v>69</v>
+      </c>
+      <c r="D24" s="2">
+        <v>60011</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="2">
+        <v>69</v>
+      </c>
+      <c r="D25" s="2">
+        <v>60012</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>